<commit_message>
Correções finais em documentos de especificações
</commit_message>
<xml_diff>
--- a/Apresentaçao Final/Gestão de Riscos.xlsx
+++ b/Apresentaçao Final/Gestão de Riscos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de probabilidade e impacto" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,7 +41,7 @@
     <t xml:space="preserve">É considerado alto, quando o risco em questão, provocar mudanças no custo e no prazo do projeto, podendo causar até mesmo o cancelamento do projeto.</t>
   </si>
   <si>
-    <t xml:space="preserve">É considerado médio, quando o risco em questão, afetar o prazo do projeto.</t>
+    <t xml:space="preserve">É considerado médio, quando o risco em questão, afetar qualidade do produto final.</t>
   </si>
   <si>
     <t xml:space="preserve">X</t>
@@ -569,26 +569,26 @@
   </sheetPr>
   <dimension ref="B2:O21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.3522267206478"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="26" min="16" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.7813765182186"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1735,23 +1735,23 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="26" min="12" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.7813765182186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>